<commit_message>
added more filters to findHutIDs
</commit_message>
<xml_diff>
--- a/HutInfo.xlsx
+++ b/HutInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ab62753a27e4e959/Projekte/SAC Scraper/FindFreeHut/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_108515955BB0510E13B93D11595ED87656CF8465" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD13AB47-73E6-41D4-B20D-8C66EEDB15B2}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_108515955BB0510E13B93D11595ED87656CF8465" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA1C6C3B-6AB7-4D2F-9DFE-4EE649FABE3B}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2055" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9480" yWindow="3210" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3878,6 +3878,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4167,11 +4171,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E320"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
-      <selection activeCell="R172" sqref="R172"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="45.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>